<commit_message>
Updated Zeitplan, diary and dbschema
</commit_message>
<xml_diff>
--- a/doc/Zeitplan.xlsx
+++ b/doc/Zeitplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t xml:space="preserve">Woche</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Datenbank, Import IST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RBAC, Auditing</t>
   </si>
   <si>
     <t xml:space="preserve">SOLL Zustand auf CSV, SOLL Zustand anhand von Events</t>
@@ -71,6 +74,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -92,6 +96,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -169,14 +174,14 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,13 +224,16 @@
       <c r="B5" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>43</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -238,7 +246,7 @@
         <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -251,7 +259,7 @@
         <v>47</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,7 +267,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -267,7 +275,7 @@
         <v>49</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,7 +283,7 @@
         <v>50</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -283,7 +291,7 @@
         <v>51</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>